<commit_message>
05/07/22 - Saliendo del trabajo
</commit_message>
<xml_diff>
--- a/2-PERSONAL/----PENDIENTES/6-RECLAMOS/7. JULIO-2022 RECLAMO BONO.xlsx
+++ b/2-PERSONAL/----PENDIENTES/6-RECLAMOS/7. JULIO-2022 RECLAMO BONO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AKM\2-PERSONAL\----PENDIENTES\6-RECLAMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9906017D-FE84-4E92-B132-46FC20F9E574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD877A-88F2-40BA-937B-0449949FBB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$7</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$8</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
   <si>
     <t>APELLIDO</t>
   </si>
@@ -102,6 +102,24 @@
   </si>
   <si>
     <t>LUPE AMPARO</t>
+  </si>
+  <si>
+    <t>BALCAZAR CORI</t>
+  </si>
+  <si>
+    <t>ANGELICA MARIA</t>
+  </si>
+  <si>
+    <t>BOLETA</t>
+  </si>
+  <si>
+    <t>Boleta indica 10 dias menos que tareo</t>
+  </si>
+  <si>
+    <t>SANCHEZ CABRERA</t>
+  </si>
+  <si>
+    <t>MERCEDES</t>
   </si>
 </sst>
 </file>
@@ -488,10 +506,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>44746</v>
       </c>
@@ -649,22 +667,67 @@
       </c>
     </row>
     <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
+      <c r="A7" s="7">
+        <v>44747</v>
+      </c>
       <c r="B7" s="8">
         <v>5</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
+      <c r="C7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="8">
+        <v>44007676</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>44747</v>
+      </c>
+      <c r="B8" s="8">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="6">
+        <v>41996696</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:H7" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <autoFilter ref="A2:H8" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <dateGroupItem year="2022" month="7" day="5" dateTimeGrouping="day"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="2">
       <filters>
-        <filter val="AQUITUARI CALDERON"/>
+        <filter val="SANCHEZ CABRERA"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
09/07/22 - Saliendo del trabajo
</commit_message>
<xml_diff>
--- a/2-PERSONAL/----PENDIENTES/6-RECLAMOS/7. JULIO-2022 RECLAMO BONO.xlsx
+++ b/2-PERSONAL/----PENDIENTES/6-RECLAMOS/7. JULIO-2022 RECLAMO BONO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AKM\2-PERSONAL\----PENDIENTES\6-RECLAMOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEFD877A-88F2-40BA-937B-0449949FBB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C1DB8B-AA6A-4D12-9C2F-F3C17A60D210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$H$9</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>APELLIDO</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>MERCEDES</t>
+  </si>
+  <si>
+    <t>PILLACA RIVERA</t>
+  </si>
+  <si>
+    <t>CANDY VANESSA</t>
   </si>
 </sst>
 </file>
@@ -506,10 +512,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,7 +698,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>44747</v>
       </c>
@@ -718,16 +724,37 @@
         <v>16</v>
       </c>
     </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>44751</v>
+      </c>
+      <c r="B9" s="8">
+        <v>7</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="6">
+        <v>73908404</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:H8" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters>
-        <dateGroupItem year="2022" month="7" day="5" dateTimeGrouping="day"/>
-      </filters>
-    </filterColumn>
+  <autoFilter ref="A2:H9" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="SANCHEZ CABRERA"/>
+        <filter val="PILLACA RIVERA"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>